<commit_message>
added Pineda 406 schedule
</commit_message>
<xml_diff>
--- a/data/horarios/horarios-21-04.raw.xlsx
+++ b/data/horarios/horarios-21-04.raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Documents\GitHub\fcc-pregrado-horarios-y-matriculas-xlsx-to-json\data\horarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5275BFD1-C81B-46A9-A31B-C8B1EEAD4A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DBB247-3CBF-4480-BC15-00EDB405ABCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{1327F3A6-D9A6-461D-B625-CF0BE3FF492C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{1327F3A6-D9A6-461D-B625-CF0BE3FF492C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1420,22 +1420,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{417C7F3C-8601-413F-8460-5E71DD68BE2F}" name="Table2" displayName="Table2" ref="A1:R512" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <autoFilter ref="A1:R512" xr:uid="{417C7F3C-8601-413F-8460-5E71DD68BE2F}">
-    <filterColumn colId="1">
+    <filterColumn colId="11">
       <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="C"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="9">
-      <filters>
-        <filter val="SJL 01-M"/>
-        <filter val="SJL 01-T"/>
-        <filter val="SJL 02-T"/>
-        <filter val="SJL 03-T"/>
+        <filter val="PINEDA YAROS WILVER"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1785,8 +1772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76592998-DD56-44F1-8DD2-864C0839338E}">
   <dimension ref="A1:R512"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Q366" sqref="Q366"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection sqref="A1:R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12245,7 +12232,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="239" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>2022</v>
       </c>
@@ -15249,7 +15236,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="307" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>2022</v>
       </c>
@@ -17337,7 +17324,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="355" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>2022</v>
       </c>
@@ -17381,7 +17368,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="356" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>2023</v>
       </c>
@@ -17425,7 +17412,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="357" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>2018</v>
       </c>
@@ -17818,7 +17805,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="366" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366">
         <v>2022</v>
       </c>
@@ -17988,7 +17975,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="370" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>2022</v>
       </c>
@@ -18293,7 +18280,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="377" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377">
         <v>2022</v>
       </c>
@@ -18334,7 +18321,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="378" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>2022</v>
       </c>
@@ -18378,7 +18365,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="379" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379">
         <v>2022</v>
       </c>
@@ -19727,7 +19714,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="410" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410">
         <v>2022</v>
       </c>

</xml_diff>